<commit_message>
dynmic json image added
</commit_message>
<xml_diff>
--- a/IDP2 Tasks tracker.xlsx
+++ b/IDP2 Tasks tracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="7610" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="7610"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="253">
   <si>
     <t>Task No.</t>
   </si>
@@ -804,6 +804,30 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>extra page coming in export</t>
+  </si>
+  <si>
+    <t>extra space</t>
+  </si>
+  <si>
+    <t>APS will share sample. More data required in json</t>
+  </si>
+  <si>
+    <t>requirement is user selected column will create multiple columns based in data</t>
+  </si>
+  <si>
+    <t>completed with demo</t>
+  </si>
+  <si>
+    <t>for more dynamic need to add section wise conditional break</t>
+  </si>
+  <si>
+    <t>it should work in textbox also.  APS will share sample</t>
+  </si>
+  <si>
+    <t>it should work in textbox also. Subtotal/summery bug coming.  APS will share sample</t>
   </si>
 </sst>
 </file>
@@ -841,7 +865,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -857,6 +881,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -908,7 +944,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -937,6 +973,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1219,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView topLeftCell="C58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C64" sqref="A64:XFD64"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1460,26 +1516,26 @@
         <v>230</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
+    <row r="11" spans="1:8" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="11" t="s">
         <v>231</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3" t="s">
-        <v>229</v>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -1776,27 +1832,27 @@
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="A25" s="2">
+    <row r="25" spans="1:8" s="13" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A25" s="10">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3" t="s">
+      <c r="G25" s="11"/>
+      <c r="H25" s="11" t="s">
         <v>229</v>
       </c>
     </row>
@@ -2094,45 +2150,49 @@
         <v>230</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="2">
+    <row r="39" spans="1:8" s="13" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="10">
         <v>38</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3" t="s">
+      <c r="E39" s="11"/>
+      <c r="F39" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="2">
+    <row r="40" spans="1:8" s="13" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="10">
         <v>39</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3" t="s">
+      <c r="F40" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11" t="s">
         <v>229</v>
       </c>
     </row>
@@ -2178,25 +2238,25 @@
         <v>229</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="2">
+    <row r="43" spans="1:8" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A43" s="10">
         <v>42</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3" t="s">
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11" t="s">
         <v>241</v>
       </c>
     </row>
@@ -2222,27 +2282,27 @@
         <v>230</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A45" s="2">
+    <row r="45" spans="1:8" s="13" customFormat="1" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="10">
         <v>44</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3" t="s">
+      <c r="F45" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11" t="s">
         <v>242</v>
       </c>
     </row>
@@ -2394,25 +2454,27 @@
         <v>230</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="2">
+    <row r="53" spans="1:8" s="13" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="10">
         <v>52</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3" t="s">
+      <c r="C53" s="11"/>
+      <c r="D53" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F53" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3" t="s">
+      <c r="G53" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="H53" s="11" t="s">
         <v>229</v>
       </c>
     </row>
@@ -2512,25 +2574,25 @@
         <v>230</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A59" s="2">
+    <row r="59" spans="1:8" s="13" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A59" s="10">
         <v>58</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="E59" s="8" t="s">
+      <c r="E59" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3" t="s">
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11" t="s">
         <v>229</v>
       </c>
     </row>
@@ -2574,27 +2636,29 @@
         <v>230</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A62" s="2">
+    <row r="62" spans="1:8" s="13" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A62" s="10">
         <v>61</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="F62" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3" t="s">
+      <c r="G62" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="H62" s="11" t="s">
         <v>242</v>
       </c>
     </row>
@@ -2890,10 +2954,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2923,82 +2987,32 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>15</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
-        <v>24</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>244</v>
-      </c>
-    </row>
     <row r="4" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>127</v>
+        <v>66</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+        <v>116</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>246</v>
+      </c>
       <c r="H4" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="16" t="s">
         <v>244</v>
       </c>
     </row>
@@ -3015,7 +3029,9 @@
       <c r="D5" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>247</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
@@ -3025,7 +3041,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>39</v>
       </c>
@@ -3072,30 +3088,6 @@
         <v>244</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>44</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
     <row r="9" spans="1:9" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>52</v>
@@ -3121,29 +3113,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
-        <v>58</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>59</v>
       </c>
@@ -3218,6 +3188,106 @@
         <v>244</v>
       </c>
     </row>
+    <row r="15" spans="1:9" s="17" customFormat="1" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="14">
+        <v>29</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="116" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>58</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="1:9" ht="174" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>44</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>244</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>